<commit_message>
first numerical test of simulator
</commit_message>
<xml_diff>
--- a/admin/ArbeitRechercheProtokoll.xlsx
+++ b/admin/ArbeitRechercheProtokoll.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseb0rn/Documents/repos/Maturaarbeit-AlgoSkitour/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA99CD0-22D6-2747-B34B-641BDEF04BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D017A95F-EB3E-DF4D-B4CD-BC14D384A4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19560" xr2:uid="{2D008D72-86D5-EB40-AD94-69D6209CD82B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Datum</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>Physiksimulation nachlesen</t>
+  </si>
+  <si>
+    <t>Physikalische grundlagen verstehen, ableiten</t>
+  </si>
+  <si>
+    <t>Physiksimulation implementieren</t>
+  </si>
+  <si>
+    <t>Vorher</t>
+  </si>
+  <si>
+    <t>Einlesen von GEOTIFF / Höhenmodell</t>
   </si>
 </sst>
 </file>
@@ -280,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -667,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D782E287-958A-6A4A-8571-1A1F19BBDAF3}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="64" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -688,99 +700,123 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>45373</v>
+      <c r="A2" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>45376</v>
+        <v>45373</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
-        <v>45377</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>45376</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>45378</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>38</v>
+        <v>45377</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <v>45378</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>45381</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="8" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>45418</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
+        <v>45418</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>45419</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>45420</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
+        <v>45420</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
         <v>45422</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>45425</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>45426</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>45427</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>45428</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scripts and production of rgb dem fro 3d map
</commit_message>
<xml_diff>
--- a/admin/ArbeitRechercheProtokoll.xlsx
+++ b/admin/ArbeitRechercheProtokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseb0rn/Documents/repos/Maturaarbeit-AlgoSkitour/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D017A95F-EB3E-DF4D-B4CD-BC14D384A4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27332BA2-2CC4-6347-A753-583DFF2181F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19560" xr2:uid="{2D008D72-86D5-EB40-AD94-69D6209CD82B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Datum</t>
   </si>
@@ -209,6 +209,13 @@
   </si>
   <si>
     <t>Einlesen von GEOTIFF / Höhenmodell</t>
+  </si>
+  <si>
+    <t>Bis hierhin auf versch. Wege mit Physiksim rumgepröbelt, nicht erfolgreich --&gt; Rein analytisches Vorgehen
+Herunterladen von schweizer geodatene, zusammenhängen in eine grosse datei, reprojezieren von bessel auf wgs84 und RGB Format, darstellung in Visualisierung. Erstmals sind 3d- Landschaften in der Schweiz dargestellt</t>
+  </si>
+  <si>
+    <t>Herunterladen von weiteren Kantonen, konvertieren und erste versuche mit webhosting auf öffentlichem server</t>
   </si>
 </sst>
 </file>
@@ -292,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -679,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D782E287-958A-6A4A-8571-1A1F19BBDAF3}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="64" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -817,6 +824,22 @@
       </c>
       <c r="B16" s="2" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>45439</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>45440</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
process dem into cost frist draft
</commit_message>
<xml_diff>
--- a/admin/ArbeitRechercheProtokoll.xlsx
+++ b/admin/ArbeitRechercheProtokoll.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseb0rn/Documents/repos/Maturaarbeit-AlgoSkitour/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8773B872-F03F-514E-BBF8-1829B46AA766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CF3FC8-D78D-3742-9B99-0614AE7D8C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19560" xr2:uid="{2D008D72-86D5-EB40-AD94-69D6209CD82B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Datum</t>
   </si>
@@ -221,6 +221,11 @@
     <t>Bis Hier seit letztem Eintrag: Neuen Servercode geschrieben, um MBTiles statisch zu hosten (Y-Koordinate anders als dateibaum),
 Kartenmaterial von Swisstopo anstelle geklauten FatMap karten, Vektorkarten eingepflegt
 Erste Versuche mit Frontend. Erreichbar unter https://robofactory.ch/ma/#12.97/46.39889/7.54997/33.6/51</t>
+  </si>
+  <si>
+    <t>Bis hierhin GRM neu digitalisiert (neue Gleichung, einfacher und representativer nach literatur)
+GPU code zur verarbeitung von rasterdaten geschrieben. Problem: Speicherbandbreite ist limitierender Faktor, nicht CPU
+Gefahrenkarte mittels GRM</t>
   </si>
 </sst>
 </file>
@@ -281,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -305,6 +310,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -691,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D782E287-958A-6A4A-8571-1A1F19BBDAF3}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="64" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -853,6 +861,14 @@
       </c>
       <c r="B19" s="7" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>45455</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
style wie handbuch proj
</commit_message>
<xml_diff>
--- a/admin/ArbeitRechercheProtokoll.xlsx
+++ b/admin/ArbeitRechercheProtokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesseb0rn/Documents/repos/Maturaarbeit-AlgoSkitour/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9D1BBB-1DBF-4E48-85E6-680829AF3308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26D8626-222D-3C45-9BF4-698EE6174703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19560" xr2:uid="{2D008D72-86D5-EB40-AD94-69D6209CD82B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Datum</t>
   </si>
@@ -333,6 +333,15 @@
     <t>Das neue selbstgeschriebene Plugin um grass igs' r_walk zu ersetzen ist Fertig.
 Arbeit an CI/CD Pipeline "automatisches Veröffentlichen"
 Findung von Modelparametern</t>
+  </si>
+  <si>
+    <t>Schreiben an Einleitung</t>
+  </si>
+  <si>
+    <t>Bis 11.8.24</t>
+  </si>
+  <si>
+    <t>Schreiben an Theorieteil und Methodik</t>
   </si>
 </sst>
 </file>
@@ -807,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D782E287-958A-6A4A-8571-1A1F19BBDAF3}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="64" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1045,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -1049,6 +1058,22 @@
       </c>
       <c r="B29" s="7" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>45509</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>